<commit_message>
update import product detail table format.xlsx (import maks 10000 row berikutnya)
</commit_message>
<xml_diff>
--- a/public/daftar product detail yang di skip.xlsx
+++ b/public/daftar product detail yang di skip.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="18">
   <si>
     <t>Table Product Detail</t>
   </si>
@@ -193,10 +193,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -227,7 +227,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -238,7 +238,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>4</v>
@@ -249,7 +249,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
@@ -260,7 +260,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>4</v>
@@ -271,10 +271,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>5</v>
@@ -282,7 +282,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
@@ -293,7 +293,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>6</v>
@@ -304,7 +304,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>6</v>
@@ -315,7 +315,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>6</v>
@@ -326,10 +326,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>5</v>
@@ -337,7 +337,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>7</v>
@@ -348,7 +348,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>7</v>
@@ -359,7 +359,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>7</v>
@@ -370,7 +370,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>7</v>
@@ -381,10 +381,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>5</v>
@@ -392,7 +392,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>8</v>
@@ -403,7 +403,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>8</v>
@@ -414,7 +414,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>8</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>8</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>5</v>
@@ -447,7 +447,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>9</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>9</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>9</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>9</v>
@@ -491,10 +491,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>5</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>10</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>10</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>10</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>10</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>5</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>11</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>11</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>11</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>11</v>
@@ -601,10 +601,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>5</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>12</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>12</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>12</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>12</v>
@@ -656,10 +656,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>5</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>13</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>13</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>13</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>13</v>
@@ -711,10 +711,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>5</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>14</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>14</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>14</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>14</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>5</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>15</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>15</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>15</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>15</v>
@@ -821,10 +821,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>5</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>16</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>16</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>16</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>16</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>5</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>17</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>17</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>17</v>
@@ -920,23 +920,12 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>